<commit_message>
1. event_dttm 추가 : done 2. 중복제거 로직 개선 : done
</commit_message>
<xml_diff>
--- a/result/log_analysis_combined.xlsx
+++ b/result/log_analysis_combined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,35 +441,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>log_time</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>page_id</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>click_type</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>act_type</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>click_text</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>keys_combined</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>values_combined</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>key_count</t>
         </is>
@@ -481,36 +486,41 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>2025-06-04 21:45:55</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>challenge/home</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>상세 챌린지</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>click</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>3일차 이런 챌린지 어때요?</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>channel, mainTitle, list_index, challengeName, challengeSeq, list_title, chal_index, activeParticipantCount, sticker</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Rround, 업로드, 0, 업로드, Optional(104), 업로드, 0, Optional(19), RECOMMEND</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>9</v>
+          <t>channel, mainTitle, click_text, list_index, challengeName, challengeSeq, list_title, chal_index, activeParticipantCount, sticker</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Rround, 업로드, 3일차 이런 챌린지 어때요?, 0, 업로드, Optional(104), 업로드, 0, Optional(19), RECOMMEND</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -519,36 +529,41 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>2025-06-04 21:45:55</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>challenge/home</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>상세 챌린지</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>click</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>이런 챌린지 어때요?</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>channel, mainTitle, list_index, challengeName, challengeSeq, list_title, chal_index, activeParticipantCount, sticker</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Rround, 업로드, 0, 업로드, Optional(104), 업로드, 0, Optional(19), RECOMMEND</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>9</v>
+          <t>channel, mainTitle, click_text, list_index, challengeName, challengeSeq, list_title, chal_index, activeParticipantCount, sticker</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Rround, 업로드, 이런 챌린지 어때요?, 0, 업로드, Optional(104), 업로드, 0, Optional(19), RECOMMEND</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -557,27 +572,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>2025-06-04 21:45:55</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>challenge/challenge_detail</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>pageview</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
         <is>
           <t xml:space="preserve">channel, activeParticipantCount, totalFeedCount, profileSeq, challengeName </t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Rround, Optional(19), Optional(31), Optional(627), 업로드</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -587,36 +607,41 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>2025-06-04 21:45:59</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>challenge/challenge_detail</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>CTA</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>click</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>클릭 텍스트</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>channel, cta_text</t>
-        </is>
-      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Rround, 인증하기</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
+          <t>channel, click_text, cta_text</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Rround, 클릭 텍스트, 인증하기</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -625,36 +650,41 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>2025-06-04 21:46:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>challenge/challenge_detail</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>상품 태그</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>popup_click</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>클릭 텍스트</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>goodsId, prd_name, channel, cta_text</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2655, 660, 정관장 홍삼대정 (홍삼대정 250g * 3병), [델리스푼] 브이핏 프리미엄 이너뷰티, Rround, 상품 선택 완료</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>4</v>
+          <t>click_text, goodsId, prd_name, channel, cta_text</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>클릭 텍스트, 2655, 660, 정관장 홍삼대정 (홍삼대정 250g * 3병), [델리스푼] 브이핏 프리미엄 이너뷰티, Rround, 상품 선택 완료</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -663,27 +693,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>2025-06-04 21:46:21</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>challenge/challenge_detail</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
         <is>
           <t>popup_imp</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
         <is>
           <t>channel, popup_title, popup_msg</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Rround, 인증 완료!, 다른 챌린지도 인증하고베스트 챌린저에 도전하세요 👏</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>3</v>
       </c>
     </row>
@@ -693,27 +728,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>2025-06-04 21:46:21</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>challenge/challenge_detail</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
         <is>
           <t>pageview</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
         <is>
           <t>profileSeq, challengeName , activeParticipantCount, totalFeedCount, channel</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Optional(627), 업로드, Optional(20), Optional(32), Rround</t>
         </is>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -723,36 +763,41 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>2025-06-04 21:46:25</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>challenge/challenge_detail</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>챌린지 상세</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>popup_click</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>클릭 텍스트</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>channel, popup_msg, cta_text, popup_title</t>
-        </is>
-      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Rround, 다른 챌린지도 인증하고베스트 챌린저에 도전하세요 👏, 확인, 인증 완료!</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>4</v>
+          <t>channel, click_text, popup_msg, cta_text, popup_title</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Rround, 클릭 텍스트, 다른 챌린지도 인증하고베스트 챌린저에 도전하세요 👏, 확인, 인증 완료!</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. QA tester 완료
</commit_message>
<xml_diff>
--- a/result/log_analysis_combined.xlsx
+++ b/result/log_analysis_combined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,28 +481,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>onboarding/carrier</t>
+          <t>life-dev/main</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>pageview</t>
+          <t>impression</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, os_name, impression_type</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, iOS, 검색 창</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -511,28 +511,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>onboarding/name</t>
+          <t>life-dev/main</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>pageview</t>
+          <t>impression</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, banner_text, banner_position, os_name, impression_type</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, ______포인트 12,500원 놓치고 있어요!___전국 날씨특파원, 오늘 날씨는?___여름맞이 체력 증진! 오운완 챌린지___, 라이프 메인 상단 카드 배너, iOS, 메인 상단 카드 배너</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -541,7 +541,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>onboarding/birth</t>
+          <t>life-dev/main</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -553,16 +553,16 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, os_name</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, iOS</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -571,28 +571,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>onboarding/terms</t>
+          <t>life-dev/main</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>pageview</t>
+          <t>swipe</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, swipe_area, swipe_direct, os_name</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 메인 상단 카드 배너, left, iOS</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -601,28 +601,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>onboarding/auth_bridge</t>
+          <t>life-dev/main</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>pageview</t>
+          <t>swipe</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, swipe_area, swipe_direct, os_name</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 메인 상단 카드 배너, left, iOS</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -631,36 +631,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>onboarding/auth_bridge</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>인증하기</t>
-        </is>
-      </c>
+          <t>life-dev/main</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>click</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>인증하기</t>
-        </is>
-      </c>
+          <t>swipe</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>channel, click_text</t>
+          <t>channel, page_url, swipe_area, swipe_direct, os_name</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Rround, 인증하기</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 메인 상단 카드 배너, left, iOS</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -669,28 +661,28 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>onboarding/auth_number</t>
+          <t>life-dev/main</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>pageview</t>
+          <t>swipe</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, swipe_area, swipe_direct, os_name</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 메인 상단 카드 배너, left, iOS</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -699,28 +691,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>splash</t>
+          <t>ecommerce-dev/product/detail/800</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>pageview</t>
+          <t>click</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, tab_name, prd_code, prd_name, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, os_name</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/product/detail/800, 상품상세
+, 800, 여성용 스킨핏 50수 투톤 모달 팬티 5P SET, 20,000원, 20,000원, 10%, 0, 0, #여성팬티___#50수팬티___#숙녀팬티___#여자팬티___#팬티세트___#모달팬티___#투톤팬티___#팬티, iOS</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -729,28 +722,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>onboarding/terms</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
+          <t>life-dev/main</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>상품 찜하기</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>pageview</t>
+          <t>click</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, prd_code, prd_name, prd_brand, prd_price_final, prd_is_ad, os_name</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 800, 여성용 스킨핏 50수 투톤 모달 팬티 5P SET, 마이그스토어, 20,000원, F, iOS</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -759,28 +756,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>onboarding/phone_number</t>
+          <t>life-dev/main</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>pageview</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>상품 더보기</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, click_text, module_id, module_order, module_name, os_name</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 상품 더보기, C-3, 33, commerce-category-ranking, iOS</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
@@ -789,36 +790,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>onboarding/start</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>로그인방법</t>
-        </is>
-      </c>
+          <t>ecommerce-dev/category/detail/543</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>click</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>kakao</t>
-        </is>
-      </c>
+          <t>pageview</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>channel, click_text</t>
+          <t>channel, page_url, ctgr_id, os_name</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Rround, kakao</t>
+          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/category/detail/543, 543, iOS</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -827,28 +820,36 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>onboarding/carrier</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
+          <t>life-dev/main</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>상품</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>pageview</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>드시모네 베이비스텝2 100억 생유산균 2박스</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel, page_url, click_text, module_id, module_order, prd_order, prd_code, prd_name, prd_brand, prd_price_final, prd_is_ad, el_order, module_name, os_name</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Rround</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 드시모네 베이비스텝2 100억 생유산균 2박스, C-3, 33, 2, 1030, 드시모네 베이비스텝2 100억 생유산균 2박스, 마이그스토어, 96,000원, F, 2, commerce-category-ranking, iOS</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -857,104 +858,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>life/feed/discovery</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>탭</t>
-        </is>
-      </c>
+          <t>ecommerce-dev/product/detail/1030</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>click</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>발견</t>
-        </is>
-      </c>
+          <t>pageview</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>channel, click_text</t>
+          <t>channel, page_url, prd_code, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, os_name</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Rround, 발견</t>
+          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/product/detail/1030, 1030, 96,000원, 86,400원, 10%, 0, 0, #프로바이오틱스___#식품___#영양제___#드시모네___#베이비스텝___#박스___#생유산균___#건강식품, iOS</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>life/feed/discovery</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>탭</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>click</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>발견</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>channel, click_text</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Rround, 발견</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>life/feed/discovery</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>pageview</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Rround</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. v05 parse 추가 1-1. value 내 쉼표 제거 기능 추가. 2. v04 tester 수정 2-1. 상수 key 값 pass 처리 기능 추가
</commit_message>
<xml_diff>
--- a/result/log_analysis_combined.xlsx
+++ b/result/log_analysis_combined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,18 +487,18 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>impression</t>
+          <t>scroll</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>channel, page_url, os_name, impression_type</t>
+          <t>channel, page_url, scroll_rate, os_name</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, iOS, 검색 창</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 75, iOS</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -514,25 +514,33 @@
           <t>life-dev/main</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>상품</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>impression</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>(스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>channel, page_url, banner_text, banner_position, os_name, impression_type</t>
+          <t>channel, page_url, click_text, module_id, module_order, prd_order, prd_code, prd_name, prd_brand, prd_price_origin, prd_price_final, prd_disc_rate, prd_is_ad, el_order, module_name, os_name</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, ______포인트 12,500원 놓치고 있어요!___전국 날씨특파원, 오늘 날씨는?___여름맞이 체력 증진! 오운완 챌린지___, 라이프 메인 상단 카드 배너, iOS, 메인 상단 카드 배너</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, (스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P, C-3, 13, 1, 3086, (스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P, 마이그스토어, 40,000원, 20,000원, 50%, F, 1, commerce-category-ranking, iOS</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -541,7 +549,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>life-dev/main</t>
+          <t>ecommerce-dev/product/detail/3086</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -553,16 +561,16 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>channel, page_url, os_name</t>
+          <t>channel, page_url, prd_code, os_name</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, iOS</t>
+          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/product/detail/3086, 3086, iOS</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -571,28 +579,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>life-dev/main</t>
+          <t>ecommerce-dev/product/detail/3086</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>swipe</t>
+          <t>click</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>channel, page_url, swipe_area, swipe_direct, os_name</t>
+          <t>channel, page_url, prd_code, os_name</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 메인 상단 카드 배너, left, iOS</t>
+          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/product/detail/3086, 3086, iOS</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -604,25 +612,33 @@
           <t>life-dev/main</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>뉴스</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>swipe</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>[OTT랭킹] '찰떡 캐스팅' 증명한 '광장'…K무비 침체 장기화</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>channel, page_url, swipe_area, swipe_direct, os_name</t>
+          <t>channel, page_url, click_text, module_id, module_order, el_order, module_name, article_title, os_name</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 메인 상단 카드 배너, left, iOS</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, [OTT랭킹] '찰떡 캐스팅' 증명한 '광장'…K무비 침체 장기화, D-1, 14, 1, news-card, [OTT랭킹] '찰떡 캐스팅' 증명한 '광장'…K무비 침체 장기화, iOS</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -631,28 +647,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>life-dev/main</t>
+          <t>life-dev/news/detail/10736</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>swipe</t>
+          <t>click</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>channel, page_url, swipe_area, swipe_direct, os_name</t>
+          <t>channel, page_url, os_name</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 메인 상단 카드 배너, left, iOS</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/news/detail/10736, iOS</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -664,25 +680,33 @@
           <t>life-dev/main</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>상품</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>swipe</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>(스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>channel, page_url, swipe_area, swipe_direct, os_name</t>
+          <t>channel, page_url, click_text, module_id, module_order, prd_order, prd_code, prd_name, prd_brand, prd_price_origin, prd_price_final, prd_disc_rate, prd_is_ad, el_order, module_name, os_name</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 메인 상단 카드 배너, left, iOS</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, (스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P, C-3, 13, 1, 3086, (스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P, 마이그스토어, 40,000원, 20,000원, 50%, F, 1, commerce-category-ranking, iOS</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -691,29 +715,36 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ecommerce-dev/product/detail/800</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
+          <t>life-dev/main</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>뉴스</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>click</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[OTT랭킹] '찰떡 캐스팅' 증명한 '광장'…K무비 침체 장기화</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>channel, page_url, tab_name, prd_code, prd_name, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, os_name</t>
+          <t>channel, page_url, click_text, module_id, module_order, el_order, module_name, article_title, os_name</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/product/detail/800, 상품상세
-, 800, 여성용 스킨핏 50수 투톤 모달 팬티 5P SET, 20,000원, 20,000원, 10%, 0, 0, #여성팬티___#50수팬티___#숙녀팬티___#여자팬티___#팬티세트___#모달팬티___#투톤팬티___#팬티, iOS</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, [OTT랭킹] '찰떡 캐스팅' 증명한 '광장'…K무비 침체 장기화, D-1, 14, 1, news-card, [OTT랭킹] '찰떡 캐스팅' 증명한 '광장'…K무비 침체 장기화, iOS</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -722,14 +753,10 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>life-dev/main</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>상품 찜하기</t>
-        </is>
-      </c>
+          <t>life-dev/news/detail/10736</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>click</t>
@@ -738,16 +765,16 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>channel, page_url, prd_code, prd_name, prd_brand, prd_price_final, prd_is_ad, os_name</t>
+          <t>channel, page_url, os_name</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 800, 여성용 스킨핏 50수 투톤 모달 팬티 5P SET, 마이그스토어, 20,000원, F, iOS</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/news/detail/10736, iOS</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -759,7 +786,11 @@
           <t>life-dev/main</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>상품</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>click</t>
@@ -767,21 +798,21 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>상품 더보기</t>
+          <t>(스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>channel, page_url, click_text, module_id, module_order, module_name, os_name</t>
+          <t>channel, page_url, click_text, module_id, module_order, prd_order, prd_code, prd_name, prd_brand, prd_price_origin, prd_price_final, prd_disc_rate, prd_is_ad, el_order, module_name, os_name</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 상품 더보기, C-3, 33, commerce-category-ranking, iOS</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, (스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P, C-3, 13, 1, 3086, (스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P, 마이그스토어, 40,000원, 20,000원, 50%, F, 1, commerce-category-ranking, iOS</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
@@ -790,7 +821,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ecommerce-dev/category/detail/543</t>
+          <t>ecommerce-dev/product/detail/3086</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -802,16 +833,16 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>channel, page_url, ctgr_id, os_name</t>
+          <t>channel, page_url, prd_code, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, os_name</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/category/detail/543, 543, iOS</t>
+          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/product/detail/3086, 3086, 40,000원, 18,000원, 55%, 0, 0, #포도씨유___#올리브유___#소르바스___#압착오일___#엑스트라버진___#해바라기유___#카놀라유___#유기농, iOS</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -820,36 +851,29 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>life-dev/main</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>상품</t>
-        </is>
-      </c>
+          <t>ecommerce-dev/product/detail/3086</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
           <t>click</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>드시모네 베이비스텝2 100억 생유산균 2박스</t>
-        </is>
-      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>channel, page_url, click_text, module_id, module_order, prd_order, prd_code, prd_name, prd_brand, prd_price_final, prd_is_ad, el_order, module_name, os_name</t>
+          <t>channel, page_url, tab_name, prd_code, prd_name, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, os_name</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 드시모네 베이비스텝2 100억 생유산균 2박스, C-3, 33, 2, 1030, 드시모네 베이비스텝2 100억 생유산균 2박스, 마이그스토어, 96,000원, F, 2, commerce-category-ranking, iOS</t>
+          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/product/detail/3086, 상품상세
+, 3086, (스페인직수입)소르바스 포도씨유500ml 1P(스페인직수입)소르바스 포도씨유500ml 1P, 40,000원, 20,000원, 55%, 0, 0, #포도씨유___#올리브유___#소르바스___#압착오일___#엑스트라버진___#해바라기유___#카놀라유___#유기농, iOS</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -858,28 +882,66 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ecommerce-dev/product/detail/1030</t>
+          <t>life-dev/main</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>pageview</t>
+          <t>scroll</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>channel, page_url, prd_code, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, os_name</t>
+          <t>channel, page_url, scroll_rate, os_name</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Rround, https://ecommerce-dev.hectoinnovation.co.kr/product/detail/1030, 1030, 96,000원, 86,400원, 10%, 0, 0, #프로바이오틱스___#식품___#영양제___#드시모네___#베이비스텝___#박스___#생유산균___#건강식품, iOS</t>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, 75, iOS</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>10</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>life-dev/main</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>뉴스</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>K뮤지컬 통했다…'어쩌면 해피엔딩', 토니상 극본상·음악상 수상</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>channel, page_url, click_text, module_id, module_order, el_order, module_name, article_title, os_name</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Rround, https://life-dev.hectoinnovation.co.kr/main, K뮤지컬 통했다…'어쩌면 해피엔딩', 토니상 극본상·음악상 수상, D-1, 19, 1, news-card, K뮤지컬 통했다…'어쩌면 해피엔딩', 토니상 극본상·음악상 수상, iOS</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
qa tester v 06
</commit_message>
<xml_diff>
--- a/result/log_analysis_combined.xlsx
+++ b/result/log_analysis_combined.xlsx
@@ -659,36 +659,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>store/main/home</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>퀵버튼</t>
-        </is>
-      </c>
+          <t>store/favorite</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>click</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>랭킹</t>
-        </is>
-      </c>
+          <t>scroll</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>channel, page_url, click_text, el_order, os_name</t>
+          <t>channel, page_url, scroll_rate, os_name</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/main/home, 랭킹, 2, Android</t>
+          <t>Rround, https://store.rround.com/favorite?fromMypage=true&amp;tab=goods, 50, iOS</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -814,7 +806,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>비달사순 2000W 파워 로즈골드 드라이어 VSD5129K</t>
+          <t>바비리스 버터 바 스트레이트너 ST520K</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -824,8 +816,8 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/main/home, 비달사순 2000W 파워 로즈골드 드라이어 VSD5129K, 식품
-, 3, 2/7, 8001, 비달사순 2000W 파워 로즈골드 드라이어 VSD5129K, 최우수판매대리점, 34,800원, 22,900원, 34%, 무료배송, F, 3, iOS</t>
+          <t>Rround, https://store.rround.com/main/home, 바비리스 버터 바 스트레이트너 ST520K, 식품
+, 5, 1/7, 8038, 바비리스 버터 바 스트레이트너 ST520K, 최우수판매대리점, 59,000원, 26,000원, 55%, 무료배송, F, 5, iOS</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -854,17 +846,17 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>channel, page_url, tab_name, area_order, prd_code, prd_name, prd_brand, prd_price_origin, prd_price_final, prd_disc_rate, prd_is_ad, el_order, os_name</t>
+          <t>channel, page_url, area_name, tab_name, prd_order, area_order, prd_code, prd_name, prd_brand, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, prd_is_ad, el_order, os_name</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/main/home, 식품
-, 1/7, 8038, 바비리스 버터 바 스트레이트너 ST520K, 최우수판매대리점, 59,000원, 26,000원, 55%, F, 5, iOS</t>
+          <t>Rround, https://store.rround.com/main/home, 주목할 만한 상품이에요!, 식품
+, 6, 3/7, 636, 비스카 블루투스 스마트 체중계 VK-S2(블랙), 빅픽처코퍼레이션, 26,900원, 13,900원, 48%, 1, 4, 무료배송, F, 6, iOS</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -946,19 +938,23 @@
           <t>click</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>생활</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>channel, page_url, os_name</t>
+          <t>channel, page_url, click_text, srch_kwd, os_name</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/main/ranking, iOS</t>
+          <t>Rround, https://store.rround.com/main/ranking, 생활, 생활, iOS</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -1059,22 +1055,22 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>슈즈랙 신발정리대 20p</t>
+          <t>(답이답이다) 베이킹소다 액체 세탁세제 용기 3L 4개</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>channel, page_url, click_text, tab_name, prd_code, prd_name, prd_brand, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_is_ad, el_order, os_name</t>
+          <t>channel, page_url, click_text, tab_name, prd_order, prd_code, prd_name, prd_brand, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, prd_is_ad, os_name</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/main/ranking, 슈즈랙 신발정리대 20p, 홈인테리어
-, 5768, 슈즈랙 신발정리대 20p, Jeepsaram 집사람, 14,000원, 11,200원, 20%, 3, 5, F, 1, iOS</t>
+          <t>Rround, https://store.rround.com/main/ranking, (답이답이다) 베이킹소다 액체 세탁세제 용기 3L 4개, 식품
+, 2, 28, (답이답이다) 베이킹소다 액체 세탁세제 용기 3L 4개, 케이디글로벌, 16,900원, 15,900원, 5%, 32, 4.5, 무료배송, F, iOS</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19">
@@ -1099,17 +1095,17 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>channel, page_url, tab_name, prd_code, prd_name, prd_brand, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_is_ad, el_order, os_name</t>
+          <t>channel, page_url, tab_name, prd_order, prd_code, prd_name, prd_brand, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, prd_is_ad, os_name</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/main/ranking, 홈인테리어
-, 5768, 슈즈랙 신발정리대 20p, Jeepsaram 집사람, 14,000원, 11,200원, 20%, 3, 5, F, 1, iOS</t>
+          <t>Rround, https://store.rround.com/main/ranking, 식품
+, 3, 36, (답이답이다) 제습제 520ml 12개, 케이디글로벌, 12,900원, 12,200원, 5%, 3, 5, 무료배송, F, iOS</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
@@ -1198,16 +1194,16 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>channel, page_url, click_text, area_name, prd_code, prd_name, prd_brand, prd_price_origin, prd_disc_rate, prd_is_ad, os_name</t>
+          <t>channel, page_url, click_text, area_name, prd_order, prd_code, prd_name, prd_brand, prd_price_origin, prd_disc_rate, prd_is_ad, os_name</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/main/deal, [닥터포헤어] 1+1 바이오3 탈모완화 샴푸 500ml, 무더운 여름, 케어의 시작, 8070, [닥터포헤어] 1+1 바이오3 탈모완화 샴푸 500ml, 닥터포헤어, 28,900원, 9%, F, iOS</t>
+          <t>Rround, https://store.rround.com/main/deal, [닥터포헤어] 1+1 바이오3 탈모완화 샴푸 500ml, 무더운 여름, 케어의 시작, 2, 8070, [닥터포헤어] 1+1 바이오3 탈모완화 샴푸 500ml, 닥터포헤어, 28,900원, 9%, F, iOS</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
@@ -1232,16 +1228,16 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>channel, page_url, area_name, prd_code, prd_name, prd_brand, prd_price_origin, prd_disc_rate, prd_is_ad, os_name</t>
+          <t>channel, page_url, area_name, prd_order, prd_code, prd_name, prd_brand, prd_price_origin, prd_disc_rate, prd_is_ad, os_name</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/main/deal, 무더운 여름, 케어의 시작, 8070, [닥터포헤어] 1+1 바이오3 탈모완화 샴푸 500ml, 닥터포헤어, 28,900원, 9%, F, iOS</t>
+          <t>Rround, https://store.rround.com/main/deal, 무더운 여름, 케어의 시작, 3, 8067, [닥터지] 레드 블레미쉬 클리어 수딩토너 기획세트, 닥터지, 18,500원, 53%, F, iOS</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
@@ -1494,7 +1490,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>store/product/detail/5105</t>
+          <t>store/product/detail/8038</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1519,8 +1515,8 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/product/detail/5105, 구매하기, 상품상세
-, 5105, 트리밀데이즈 루테인 밀크씨슬 프리미엄 900mg*30캡슐, 15,900원, 10,800원, 32%, 0, 0, #한미양행___#CMG제약___#트리밀데이즈___#영양제___#비타민, iOS</t>
+          <t>Rround, https://store.rround.com/product/detail/8038, 구매하기, 상품상세
+, 8038, 바비리스 버터 바 스트레이트너 ST520K, 59,000원, 26,000원, 55%, 0, 0, #고데기___#고대기___#여행용고데기___#미용실고데기___#뿌리볼륨고데기___#가벼운고데기___#스트레이트너___#매직기___#바비리스고데기___#웨이브고데기___#온도조절고데기, iOS</t>
         </is>
       </c>
       <c r="H31" t="n">
@@ -1533,24 +1529,33 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>store/order/payment</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr"/>
+          <t>store/product/detail/8038</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>구매 버튼</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>pageview</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>click</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>바로 구매하기</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>channel, page_url, referer_url, prd_code, prd_name, prd_brand, total_price_origin, total_price_disc, total_price_final, total_delivery_price, use_rrpay_point, rrpay_point, os_name</t>
+          <t>channel, page_url, click_text, tab_name, prd_code, prd_name, prd_price_origin, prd_price_final, prd_disc_rate, prd_review_cnt, prd_review_score, prd_tag, os_name</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Rround, https://store.rround.com/order/payment?selectedCartId=[27035], https://store.rround.com/product/detail/5105, 5105, 트리밀데이즈 루테인 밀크씨슬 프리미엄 900mg*30캡슐, 제이앤스토어, 15,900원, -5,100원, 10,800원, 0원, -0원, 51원, iOS</t>
+          <t>Rround, https://store.rround.com/product/detail/8038, 바로 구매하기, 상품상세
+, 8038, 바비리스 버터 바 스트레이트너 ST520K, 59,000원, 26,000원, 55%, 0, 0, #고데기___#고대기___#여행용고데기___#미용실고데기___#뿌리볼륨고데기___#가벼운고데기___#스트레이트너___#매직기___#바비리스고데기___#웨이브고데기___#온도조절고데기, iOS</t>
         </is>
       </c>
       <c r="H32" t="n">

</xml_diff>